<commit_message>
Adding 'Perfadex Plus' as a permissible value for perfusion and transport solution
</commit_message>
<xml_diff>
--- a/organ/latest/organ.xlsx
+++ b/organ/latest/organ.xlsx
@@ -159,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="101">
   <si>
     <t>organ_id</t>
   </si>
@@ -218,6 +218,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000151</t>
   </si>
   <si>
+    <t>Perfadex Plus</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000249</t>
+  </si>
+  <si>
     <t>Miltenyi Tissue Preservation Buffer</t>
   </si>
   <si>
@@ -449,7 +455,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2023-08-11T13:14:30-07:00</t>
+    <t>2023-09-01T13:52:59-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -592,60 +598,60 @@
         <v>16</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2">
       <c r="V2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -657,10 +663,10 @@
       <formula1>'organ_condition'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'perfusion_solution'!$A$1:$A$6</formula1>
+      <formula1>'perfusion_solution'!$A$1:$A$7</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="F2:F1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'transport_solution'!$A$1:$A$11</formula1>
+      <formula1>'transport_solution'!$A$1:$A$12</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>0</formula1>
@@ -728,34 +734,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -773,34 +779,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -818,26 +824,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -861,30 +867,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -968,7 +974,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1022,6 +1028,14 @@
         <v>28</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -1029,7 +1043,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1037,18 +1051,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3">
@@ -1061,10 +1075,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5">
@@ -1077,34 +1091,34 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10">
@@ -1121,6 +1135,14 @@
       </c>
       <c r="B11" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1138,42 +1160,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1191,42 +1213,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1244,42 +1266,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1297,34 +1319,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating organ and sample metadata
</commit_message>
<xml_diff>
--- a/organ/latest/organ.xlsx
+++ b/organ/latest/organ.xlsx
@@ -413,7 +413,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2023-09-08T20:50:05-07:00</t>
+    <t>2023-10-05T17:09:38-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -626,49 +626,49 @@
     <dataValidation type="list" sqref="F2:F1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'transport_solution'!$A$1:$A$12</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
       <formula2/>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'warm_ischemic_time_unit'!$A$1:$A$2</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
       <formula2/>
     </dataValidation>
     <dataValidation type="list" sqref="J2:J1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'cold_ischemic_time_unit'!$A$1:$A$2</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="L2:L1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="L2:L1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
       <formula2/>
     </dataValidation>
     <dataValidation type="list" sqref="M2:M1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'weight_unit'!$A$1:$A$2</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="N2:N1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="N2:N1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
       <formula2/>
     </dataValidation>
     <dataValidation type="list" sqref="O2:O1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'height_unit'!$A$1:$A$2</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="P2:P1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="P2:P1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
       <formula2/>
     </dataValidation>
     <dataValidation type="list" sqref="Q2:Q1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'width_unit'!$A$1:$A$2</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="R2:R1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="R2:R1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
       <formula2/>
     </dataValidation>
     <dataValidation type="list" sqref="S2:S1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'length_unit'!$A$1:$A$2</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="T2:T1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="T2:T1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
       <formula2/>
     </dataValidation>

</xml_diff>